<commit_message>
automacao e analise de dados
</commit_message>
<xml_diff>
--- a/IntensivaoPythonHashtag2023/Aula 3/commodities_atualizado.xlsx
+++ b/IntensivaoPythonHashtag2023/Aula 3/commodities_atualizado.xlsx
@@ -483,7 +483,7 @@
         <v>424.37</v>
       </c>
       <c r="C5">
-        <v>429.54</v>
+        <v>429.45</v>
       </c>
       <c r="D5" t="b">
         <v>0</v>
@@ -539,7 +539,7 @@
         <v>321.77</v>
       </c>
       <c r="C9">
-        <v>329.05</v>
+        <v>328.98</v>
       </c>
       <c r="D9" t="b">
         <v>0</v>

</xml_diff>